<commit_message>
updated Hybrid Score based
</commit_message>
<xml_diff>
--- a/Homework2/Plots.xlsx
+++ b/Homework2/Plots.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="6400" yWindow="2860" windowWidth="38400" windowHeight="23540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Task 4 CBs" sheetId="1" r:id="rId1"/>
@@ -973,11 +973,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="922973008"/>
-        <c:axId val="903423968"/>
+        <c:axId val="467384032"/>
+        <c:axId val="495529872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="922973008"/>
+        <c:axId val="467384032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1098,14 +1098,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="903423968"/>
+        <c:crossAx val="495529872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20.0"/>
         <c:minorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="903423968"/>
+        <c:axId val="495529872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1218,7 +1218,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="922973008"/>
+        <c:crossAx val="467384032"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1434,6 +1434,27 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1513,6 +1534,27 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.27</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1592,6 +1634,27 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.29</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1605,11 +1668,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="904178848"/>
-        <c:axId val="903359472"/>
+        <c:axId val="474686400"/>
+        <c:axId val="474695136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="904178848"/>
+        <c:axId val="474686400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1709,12 +1772,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="903359472"/>
+        <c:crossAx val="474695136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="903359472"/>
+        <c:axId val="474695136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1807,7 +1870,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="904178848"/>
+        <c:crossAx val="474686400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1933,7 +1996,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2257,11 +2319,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="903829344"/>
-        <c:axId val="903838080"/>
+        <c:axId val="495907616"/>
+        <c:axId val="495916352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="903829344"/>
+        <c:axId val="495907616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -2315,7 +2377,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2362,14 +2423,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="903838080"/>
+        <c:crossAx val="495916352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20.0"/>
         <c:minorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="903838080"/>
+        <c:axId val="495916352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2415,7 +2476,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2462,7 +2522,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="903829344"/>
+        <c:crossAx val="495907616"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2476,7 +2536,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2588,7 +2647,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2849,11 +2907,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="923856448"/>
-        <c:axId val="923865184"/>
+        <c:axId val="467635072"/>
+        <c:axId val="467644016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="923856448"/>
+        <c:axId val="467635072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2906,7 +2964,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2953,12 +3010,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="923865184"/>
+        <c:crossAx val="467644016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="923865184"/>
+        <c:axId val="467644016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3004,7 +3061,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3051,7 +3107,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="923856448"/>
+        <c:crossAx val="467635072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3065,7 +3121,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3332,6 +3387,27 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.27</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3341,6 +3417,27 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3488,11 +3585,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="923956912"/>
-        <c:axId val="923943440"/>
+        <c:axId val="497072864"/>
+        <c:axId val="497081616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="923956912"/>
+        <c:axId val="497072864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3585,12 +3682,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="923943440"/>
+        <c:crossAx val="497081616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="923943440"/>
+        <c:axId val="497081616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3683,7 +3780,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="923956912"/>
+        <c:crossAx val="497072864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4761,7 +4858,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="B3:D9"/>
+      <selection activeCell="N9" sqref="L3:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4827,9 +4924,15 @@
       <c r="K3" s="4">
         <v>1</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="L3" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0.38</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="20">
@@ -4847,9 +4950,15 @@
       <c r="K4" s="20">
         <v>3</v>
       </c>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
+      <c r="L4" s="21">
+        <v>0.36</v>
+      </c>
+      <c r="M4" s="21">
+        <v>0.35</v>
+      </c>
+      <c r="N4" s="21">
+        <v>0.36</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="22">
@@ -4867,9 +4976,15 @@
       <c r="K5" s="22">
         <v>5</v>
       </c>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
+      <c r="L5" s="23">
+        <v>0.35</v>
+      </c>
+      <c r="M5" s="23">
+        <v>0.34</v>
+      </c>
+      <c r="N5" s="23">
+        <v>0.35</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="22">
@@ -4887,9 +5002,15 @@
       <c r="K6" s="22">
         <v>10</v>
       </c>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
+      <c r="L6" s="23">
+        <v>0.34</v>
+      </c>
+      <c r="M6" s="23">
+        <v>0.33</v>
+      </c>
+      <c r="N6" s="23">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="22">
@@ -4907,9 +5028,15 @@
       <c r="K7" s="22">
         <v>20</v>
       </c>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
+      <c r="L7" s="23">
+        <v>0.32</v>
+      </c>
+      <c r="M7" s="23">
+        <v>0.32</v>
+      </c>
+      <c r="N7" s="23">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="22">
@@ -4927,9 +5054,15 @@
       <c r="K8" s="22">
         <v>50</v>
       </c>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
+      <c r="L8" s="23">
+        <v>0.31</v>
+      </c>
+      <c r="M8" s="23">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N8" s="23">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
@@ -4947,9 +5080,15 @@
       <c r="K9" s="4">
         <v>100</v>
       </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
+      <c r="L9" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0.28999999999999998</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M10" s="24"/>
@@ -5179,7 +5318,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="C9" sqref="C9:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5316,60 +5455,104 @@
       <c r="B9" s="8">
         <v>1</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
+      <c r="C9" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.38</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="32"/>
       <c r="B10" s="4">
         <v>3</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="11"/>
+      <c r="C10" s="21">
+        <v>0.36</v>
+      </c>
+      <c r="D10" s="21">
+        <v>0.35</v>
+      </c>
+      <c r="E10" s="21">
+        <v>0.36</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="32"/>
       <c r="B11" s="4">
         <v>5</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="11"/>
+      <c r="C11" s="23">
+        <v>0.35</v>
+      </c>
+      <c r="D11" s="23">
+        <v>0.34</v>
+      </c>
+      <c r="E11" s="23">
+        <v>0.35</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="32"/>
       <c r="B12" s="4">
         <v>10</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="11"/>
+      <c r="C12" s="23">
+        <v>0.34</v>
+      </c>
+      <c r="D12" s="23">
+        <v>0.33</v>
+      </c>
+      <c r="E12" s="23">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="32"/>
       <c r="B13" s="4">
         <v>20</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="11"/>
+      <c r="C13" s="23">
+        <v>0.32</v>
+      </c>
+      <c r="D13" s="23">
+        <v>0.32</v>
+      </c>
+      <c r="E13" s="23">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33"/>
       <c r="B14" s="12">
         <v>50</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
+      <c r="C14" s="23">
+        <v>0.31</v>
+      </c>
+      <c r="D14" s="23">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E14" s="23">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="25">
         <v>100</v>
       </c>
-      <c r="C15" s="26"/>
+      <c r="C15" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.28999999999999998</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="31" t="s">

</xml_diff>

<commit_message>
Report: Task2 Documentation done
</commit_message>
<xml_diff>
--- a/Homework2/Plots.xlsx
+++ b/Homework2/Plots.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="2860" windowWidth="38400" windowHeight="23540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="49880" windowHeight="28340" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Task 4 CBs" sheetId="1" r:id="rId1"/>
@@ -629,7 +629,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -973,11 +972,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="467384032"/>
-        <c:axId val="495529872"/>
+        <c:axId val="913074448"/>
+        <c:axId val="949449984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="467384032"/>
+        <c:axId val="913074448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1031,7 +1030,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1098,14 +1096,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="495529872"/>
+        <c:crossAx val="949449984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20.0"/>
         <c:minorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="495529872"/>
+        <c:axId val="949449984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1151,7 +1149,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1218,7 +1215,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="467384032"/>
+        <c:crossAx val="913074448"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1232,7 +1229,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1344,7 +1340,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1668,11 +1663,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="474686400"/>
-        <c:axId val="474695136"/>
+        <c:axId val="948803792"/>
+        <c:axId val="948812448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="474686400"/>
+        <c:axId val="948803792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1725,7 +1720,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1772,12 +1766,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474695136"/>
+        <c:crossAx val="948812448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="474695136"/>
+        <c:axId val="948812448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1823,7 +1817,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1870,7 +1863,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474686400"/>
+        <c:crossAx val="948803792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1884,7 +1877,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2319,11 +2311,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="495907616"/>
-        <c:axId val="495916352"/>
+        <c:axId val="949662976"/>
+        <c:axId val="949671712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="495907616"/>
+        <c:axId val="949662976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -2423,14 +2415,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="495916352"/>
+        <c:crossAx val="949671712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20.0"/>
         <c:minorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="495916352"/>
+        <c:axId val="949671712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2522,7 +2514,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="495907616"/>
+        <c:crossAx val="949662976"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2907,11 +2899,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="467635072"/>
-        <c:axId val="467644016"/>
+        <c:axId val="949750672"/>
+        <c:axId val="949759408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="467635072"/>
+        <c:axId val="949750672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3010,12 +3002,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="467644016"/>
+        <c:crossAx val="949759408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="467644016"/>
+        <c:axId val="949759408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3107,7 +3099,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="467635072"/>
+        <c:crossAx val="949750672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3585,11 +3577,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="497072864"/>
-        <c:axId val="497081616"/>
+        <c:axId val="949863472"/>
+        <c:axId val="949872224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="497072864"/>
+        <c:axId val="949863472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3682,12 +3674,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497081616"/>
+        <c:crossAx val="949872224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="497081616"/>
+        <c:axId val="949872224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3780,7 +3772,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497072864"/>
+        <c:crossAx val="949863472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5318,7 +5310,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:E15"/>
+      <selection activeCell="T36" sqref="T36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated report + plot
</commit_message>
<xml_diff>
--- a/Homework2/Plots.xlsx
+++ b/Homework2/Plots.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="49880" windowHeight="28340" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="49880" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Task 4 CBs" sheetId="1" r:id="rId1"/>
     <sheet name="Task 4 Hybrids" sheetId="8" r:id="rId2"/>
     <sheet name="Task3 Vergleich alle" sheetId="4" r:id="rId3"/>
+    <sheet name="Language Stats" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>MAP</t>
   </si>
@@ -65,6 +66,138 @@
   </si>
   <si>
     <t>UNSER HR SCB Wiki</t>
+  </si>
+  <si>
+    <t>af</t>
+  </si>
+  <si>
+    <t>sw</t>
+  </si>
+  <si>
+    <t>ca</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>cy</t>
+  </si>
+  <si>
+    <t>cs</t>
+  </si>
+  <si>
+    <t>et</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>ru</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>tr</t>
+  </si>
+  <si>
+    <t>lt</t>
+  </si>
+  <si>
+    <t>lv</t>
+  </si>
+  <si>
+    <t>tl</t>
+  </si>
+  <si>
+    <t>vi</t>
+  </si>
+  <si>
+    <t>ro</t>
+  </si>
+  <si>
+    <t>pl</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>hr</t>
+  </si>
+  <si>
+    <t>bn</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>fa</t>
+  </si>
+  <si>
+    <t>fi</t>
+  </si>
+  <si>
+    <t>hu</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>he</t>
+  </si>
+  <si>
+    <t>sq</t>
+  </si>
+  <si>
+    <t>ko</t>
+  </si>
+  <si>
+    <t>sv</t>
+  </si>
+  <si>
+    <t>ur</t>
+  </si>
+  <si>
+    <t>sk</t>
+  </si>
+  <si>
+    <t>so</t>
+  </si>
+  <si>
+    <t>uk</t>
+  </si>
+  <si>
+    <t>sl</t>
+  </si>
+  <si>
+    <t>cn</t>
+  </si>
+  <si>
+    <t>Englisch (45341)</t>
+  </si>
+  <si>
+    <t>Deutsch (1000)</t>
+  </si>
+  <si>
+    <t>Spanisch (842)</t>
+  </si>
+  <si>
+    <t>Portugiesisch (754)</t>
+  </si>
+  <si>
+    <t>Andere (3386)</t>
+  </si>
+  <si>
+    <t>Termsvergleich</t>
+  </si>
+  <si>
+    <t>Musixmatch</t>
+  </si>
+  <si>
+    <t>Wikipedia</t>
   </si>
 </sst>
 </file>
@@ -429,8 +562,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -538,7 +675,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -553,6 +690,8 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -567,6 +706,8 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -629,6 +770,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -709,25 +851,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.0</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50.0</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100.0</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -739,25 +881,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.02</c:v>
+                  <c:v>0.72</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95</c:v>
+                  <c:v>0.74</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9</c:v>
+                  <c:v>0.74</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.83</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.86</c:v>
+                  <c:v>0.73</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.94</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.89</c:v>
+                  <c:v>0.64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -809,25 +951,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.0</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50.0</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100.0</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -839,25 +981,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.5</c:v>
+                  <c:v>0.55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.57</c:v>
+                  <c:v>1.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.57</c:v>
+                  <c:v>1.54</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.41</c:v>
+                  <c:v>2.48</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.46</c:v>
+                  <c:v>4.59</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6</c:v>
+                  <c:v>7.98</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.56</c:v>
+                  <c:v>10.83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -909,25 +1051,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.0</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50.0</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100.0</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -939,25 +1081,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.45</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.39</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.33</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.26</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.24</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.27</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.38</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.32</c:v>
+                  <c:v>1.21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -972,11 +1114,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="913074448"/>
-        <c:axId val="949449984"/>
+        <c:axId val="-1485876272"/>
+        <c:axId val="-1485863872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="913074448"/>
+        <c:axId val="-1485876272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1020,16 +1162,17 @@
                   <a:rPr lang="de-DE" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>Neighbours</a:t>
+                  <a:t>Recommendet </a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="de-DE" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
-                  <a:t>  (Artists)</a:t>
+                  <a:t>Artists</a:t>
                 </a:r>
                 <a:endParaRPr lang="de-DE" sz="2000" b="1"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1096,14 +1239,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="949449984"/>
+        <c:crossAx val="-1485863872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20.0"/>
         <c:minorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="949449984"/>
+        <c:axId val="-1485863872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1149,6 +1292,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1215,7 +1359,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="913074448"/>
+        <c:crossAx val="-1485876272"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1229,6 +1373,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1340,6 +1485,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1417,9 +1563,6 @@
                 <c:pt idx="5">
                   <c:v>50.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>100.0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1430,25 +1573,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.38</c:v>
+                  <c:v>0.219</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.35</c:v>
+                  <c:v>0.22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.34</c:v>
+                  <c:v>0.22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32</c:v>
+                  <c:v>0.18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.31</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.3</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1517,9 +1657,6 @@
                 <c:pt idx="5">
                   <c:v>50.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>100.0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1530,25 +1667,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.38</c:v>
+                  <c:v>1.63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35</c:v>
+                  <c:v>4.55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.34</c:v>
+                  <c:v>7.48</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.33</c:v>
+                  <c:v>13.29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32</c:v>
+                  <c:v>19.47</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.29</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.27</c:v>
+                  <c:v>31.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1617,9 +1751,6 @@
                 <c:pt idx="5">
                   <c:v>50.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>100.0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1630,25 +1761,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.38</c:v>
+                  <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36</c:v>
+                  <c:v>0.41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.35</c:v>
+                  <c:v>0.43</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.34</c:v>
+                  <c:v>0.43</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32</c:v>
+                  <c:v>0.37</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.29</c:v>
+                  <c:v>0.31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1663,11 +1791,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="948803792"/>
-        <c:axId val="948812448"/>
+        <c:axId val="-1490078544"/>
+        <c:axId val="-1476369440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="948803792"/>
+        <c:axId val="-1490078544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1720,6 +1848,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1766,12 +1895,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="948812448"/>
+        <c:crossAx val="-1476369440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="948812448"/>
+        <c:axId val="-1476369440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1817,6 +1946,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1863,7 +1993,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="948803792"/>
+        <c:crossAx val="-1490078544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1877,6 +2007,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1988,6 +2119,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2311,11 +2443,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="949662976"/>
-        <c:axId val="949671712"/>
+        <c:axId val="-1489261376"/>
+        <c:axId val="-1489252640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="949662976"/>
+        <c:axId val="-1489261376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -2369,6 +2501,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2415,14 +2548,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="949671712"/>
+        <c:crossAx val="-1489252640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20.0"/>
         <c:minorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="949671712"/>
+        <c:axId val="-1489252640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2468,6 +2601,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2514,7 +2648,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="949662976"/>
+        <c:crossAx val="-1489261376"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2528,6 +2662,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2639,6 +2774,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2899,11 +3035,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="949750672"/>
-        <c:axId val="949759408"/>
+        <c:axId val="-1489151312"/>
+        <c:axId val="-1489142576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="949750672"/>
+        <c:axId val="-1489151312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2956,6 +3092,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3002,12 +3139,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="949759408"/>
+        <c:crossAx val="-1489142576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="949759408"/>
+        <c:axId val="-1489142576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3053,6 +3190,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3099,7 +3237,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="949750672"/>
+        <c:crossAx val="-1489151312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3113,6 +3251,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3577,11 +3716,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="949863472"/>
-        <c:axId val="949872224"/>
+        <c:axId val="-1475219456"/>
+        <c:axId val="-1475210688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="949863472"/>
+        <c:axId val="-1475219456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3674,12 +3813,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="949872224"/>
+        <c:crossAx val="-1475210688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="949872224"/>
+        <c:axId val="-1475210688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3772,7 +3911,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="949863472"/>
+        <c:crossAx val="-1475219456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3853,7 +3992,336 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprachenverteilung Musixmatch Lyrics</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Language Stats'!$E$4:$E$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Englisch (45341)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Deutsch (1000)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Spanisch (842)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Portugiesisch (754)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Andere (3386)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Language Stats'!$F$4:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>45341.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>842.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>754.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3386.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4409,6 +4877,525 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4568,6 +5555,41 @@
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks noChangeAspect="1"/>
         </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>814917</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>74083</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>481542</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>112183</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4847,10 +5869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="L3:N9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4860,7 +5882,7 @@
     <col min="5" max="5" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
         <v>4</v>
       </c>
@@ -4874,7 +5896,7 @@
       <c r="M1" s="29"/>
       <c r="N1" s="30"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -4900,189 +5922,244 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3">
-        <v>1.02</v>
+        <v>0.72</v>
       </c>
       <c r="C3" s="3">
-        <v>2.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D3" s="3">
-        <v>1.45</v>
+        <v>0.62</v>
       </c>
       <c r="K3" s="4">
         <v>1</v>
       </c>
       <c r="L3" s="3">
+        <v>0.219</v>
+      </c>
+      <c r="M3" s="3">
+        <v>1.63</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0.39</v>
+      </c>
+      <c r="P3" s="3">
         <v>0.38</v>
       </c>
-      <c r="M3" s="3">
+      <c r="Q3" s="3">
         <v>0.38</v>
       </c>
-      <c r="N3" s="3">
+      <c r="R3" s="3">
         <v>0.38</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="20">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B4" s="23">
-        <v>0.95</v>
+        <v>0.74</v>
       </c>
       <c r="C4" s="23">
-        <v>2.57</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D4" s="23">
-        <v>1.39</v>
+        <v>0.89</v>
       </c>
       <c r="K4" s="20">
         <v>3</v>
       </c>
       <c r="L4" s="21">
+        <v>0.21</v>
+      </c>
+      <c r="M4" s="21">
+        <v>4.55</v>
+      </c>
+      <c r="N4" s="21">
+        <v>0.41</v>
+      </c>
+      <c r="P4" s="21">
         <v>0.36</v>
       </c>
-      <c r="M4" s="21">
+      <c r="Q4" s="21">
         <v>0.35</v>
       </c>
-      <c r="N4" s="21">
+      <c r="R4" s="21">
         <v>0.36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="22">
-        <v>5</v>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>30</v>
       </c>
       <c r="B5" s="23">
-        <v>0.9</v>
+        <v>0.74</v>
       </c>
       <c r="C5" s="23">
-        <v>2.57</v>
+        <v>1.54</v>
       </c>
       <c r="D5" s="23">
-        <v>1.33</v>
+        <v>1</v>
       </c>
       <c r="K5" s="22">
         <v>5</v>
       </c>
       <c r="L5" s="23">
+        <v>0.22</v>
+      </c>
+      <c r="M5" s="23">
+        <v>7.48</v>
+      </c>
+      <c r="N5" s="23">
+        <v>0.43</v>
+      </c>
+      <c r="P5" s="23">
         <v>0.35</v>
       </c>
-      <c r="M5" s="23">
+      <c r="Q5" s="23">
         <v>0.34</v>
       </c>
-      <c r="N5" s="23">
+      <c r="R5" s="23">
         <v>0.35</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="22">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B6" s="23">
-        <v>0.83</v>
+        <v>0.75</v>
       </c>
       <c r="C6" s="23">
-        <v>2.41</v>
+        <v>2.48</v>
       </c>
       <c r="D6" s="23">
-        <v>1.24</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="K6" s="22">
         <v>10</v>
       </c>
       <c r="L6" s="23">
+        <v>0.22</v>
+      </c>
+      <c r="M6" s="23">
+        <v>13.29</v>
+      </c>
+      <c r="N6" s="23">
+        <v>0.43</v>
+      </c>
+      <c r="P6" s="23">
         <v>0.34</v>
       </c>
-      <c r="M6" s="23">
+      <c r="Q6" s="23">
         <v>0.33</v>
       </c>
-      <c r="N6" s="23">
+      <c r="R6" s="23">
         <v>0.34</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="22">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="B7" s="23">
-        <v>0.86</v>
+        <v>0.73</v>
       </c>
       <c r="C7" s="23">
-        <v>2.46</v>
+        <v>4.59</v>
       </c>
       <c r="D7" s="23">
-        <v>1.27</v>
+        <v>1.26</v>
       </c>
       <c r="K7" s="22">
         <v>20</v>
       </c>
       <c r="L7" s="23">
+        <v>0.18</v>
+      </c>
+      <c r="M7" s="23">
+        <v>19.47</v>
+      </c>
+      <c r="N7" s="23">
+        <v>0.37</v>
+      </c>
+      <c r="P7" s="23">
         <v>0.32</v>
       </c>
-      <c r="M7" s="23">
+      <c r="Q7" s="23">
         <v>0.32</v>
       </c>
-      <c r="N7" s="23">
+      <c r="R7" s="23">
         <v>0.32</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="22">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="B8" s="23">
-        <v>0.94</v>
+        <v>0.67</v>
       </c>
       <c r="C8" s="23">
-        <v>2.6</v>
+        <v>7.98</v>
       </c>
       <c r="D8" s="23">
-        <v>1.38</v>
+        <v>1.24</v>
       </c>
       <c r="K8" s="22">
         <v>50</v>
       </c>
       <c r="L8" s="23">
+        <v>0.16</v>
+      </c>
+      <c r="M8" s="23">
+        <v>31.01</v>
+      </c>
+      <c r="N8" s="23">
         <v>0.31</v>
       </c>
-      <c r="M8" s="23">
+      <c r="P8" s="23">
+        <v>0.31</v>
+      </c>
+      <c r="Q8" s="23">
         <v>0.28999999999999998</v>
       </c>
-      <c r="N8" s="23">
+      <c r="R8" s="23">
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
-        <v>100</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.89</v>
-      </c>
-      <c r="C9" s="3">
-        <v>2.56</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1.32</v>
-      </c>
-      <c r="K9" s="4">
-        <v>100</v>
-      </c>
-      <c r="L9" s="3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="22">
+        <v>300</v>
+      </c>
+      <c r="B9" s="23">
+        <v>0.64</v>
+      </c>
+      <c r="C9" s="23">
+        <v>10.83</v>
+      </c>
+      <c r="D9" s="23">
+        <v>1.21</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="P9" s="3">
         <v>0.3</v>
       </c>
-      <c r="M9" s="3">
+      <c r="Q9" s="3">
         <v>0.27</v>
       </c>
-      <c r="N9" s="3">
+      <c r="R9" s="3">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M10" s="24"/>
     </row>
   </sheetData>
@@ -5309,8 +6386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T36" sqref="T36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5731,4 +6808,366 @@
   </colBreaks>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:R42"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4">
+        <v>45341</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>56</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>322</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8">
+        <v>3386</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <f>SUM(F4:F8)</f>
+        <v>51323</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>163</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>54</v>
+      </c>
+      <c r="R12">
+        <v>11922</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>334</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>55</v>
+      </c>
+      <c r="R13">
+        <v>85917</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <f>SUM(C5:C40)</f>
+        <v>3386</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>